<commit_message>
Small changes to demands tab
</commit_message>
<xml_diff>
--- a/Monthly_Demand.xlsx
+++ b/Monthly_Demand.xlsx
@@ -16,7 +16,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
-    <t>Total Demand for All Users customers for 2023 (Mthembanji)</t>
+    <t>Total Demand for All Users customers for 2023 (Kudembe)</t>
   </si>
   <si>
     <t>Month</t>
@@ -430,7 +430,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>378.1793333333</v>
+        <v>375.829</v>
       </c>
     </row>
     <row r="4" spans="1:3">

</xml_diff>